<commit_message>
forgot to change that in the resource folder; changed now
</commit_message>
<xml_diff>
--- a/html/resources/testTrialLoop.xlsx
+++ b/html/resources/testTrialLoop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuan/Documents/face_loc_Mooney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2811755-16E7-824F-83F9-DE963DC21355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E58E35-F3B7-FA40-803F-8939121224C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,28 +31,28 @@
     <t>image</t>
   </si>
   <si>
-    <t>1.bmp</t>
-  </si>
-  <si>
-    <t>5.bmp</t>
-  </si>
-  <si>
-    <t>9.bmp</t>
-  </si>
-  <si>
-    <t>13.bmp</t>
-  </si>
-  <si>
-    <t>17.bmp</t>
-  </si>
-  <si>
-    <t>21.bmp</t>
-  </si>
-  <si>
-    <t>25.bmp</t>
-  </si>
-  <si>
-    <t>29.bmp</t>
+    <t>stim/1.bmp</t>
+  </si>
+  <si>
+    <t>stim/5.bmp</t>
+  </si>
+  <si>
+    <t>stim/9.bmp</t>
+  </si>
+  <si>
+    <t>stim/13.bmp</t>
+  </si>
+  <si>
+    <t>stim/17.bmp</t>
+  </si>
+  <si>
+    <t>stim/21.bmp</t>
+  </si>
+  <si>
+    <t>stim/25.bmp</t>
+  </si>
+  <si>
+    <t>stim/29.bmp</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
put images out of stim folder; also change the column name to stimFile in the loop file
</commit_message>
<xml_diff>
--- a/html/resources/testTrialLoop.xlsx
+++ b/html/resources/testTrialLoop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuan/Documents/face_loc_Mooney/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E58E35-F3B7-FA40-803F-8939121224C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67E7AA8-A312-FB4F-B32B-26AF72F411ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,31 +28,31 @@
     <t>coey</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>stim/1.bmp</t>
-  </si>
-  <si>
-    <t>stim/5.bmp</t>
-  </si>
-  <si>
-    <t>stim/9.bmp</t>
-  </si>
-  <si>
-    <t>stim/13.bmp</t>
-  </si>
-  <si>
-    <t>stim/17.bmp</t>
-  </si>
-  <si>
-    <t>stim/21.bmp</t>
-  </si>
-  <si>
-    <t>stim/25.bmp</t>
-  </si>
-  <si>
-    <t>stim/29.bmp</t>
+    <t>1.bmp</t>
+  </si>
+  <si>
+    <t>5.bmp</t>
+  </si>
+  <si>
+    <t>9.bmp</t>
+  </si>
+  <si>
+    <t>13.bmp</t>
+  </si>
+  <si>
+    <t>17.bmp</t>
+  </si>
+  <si>
+    <t>21.bmp</t>
+  </si>
+  <si>
+    <t>25.bmp</t>
+  </si>
+  <si>
+    <t>29.bmp</t>
+  </si>
+  <si>
+    <t>imageFile</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -388,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -399,7 +399,7 @@
         <v>-0.254556</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -410,7 +410,7 @@
         <v>-0.28560600000000003</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -421,7 +421,7 @@
         <v>0.21915000000000001</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -432,7 +432,7 @@
         <v>0.33258599999999999</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -443,7 +443,7 @@
         <v>0.21915000000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -454,7 +454,7 @@
         <v>0.34772399999999998</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -465,7 +465,7 @@
         <v>-0.21915000000000001</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
         <v>0.13775399999999999</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>